<commit_message>
Updated results with bo sherman
</commit_message>
<xml_diff>
--- a/races/OVCX_2_Shred The Beach.xlsx
+++ b/races/OVCX_2_Shred The Beach.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1395" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1395" uniqueCount="370">
   <si>
     <t>Race Date</t>
   </si>
@@ -872,6 +872,9 @@
   </si>
   <si>
     <t>Anderson</t>
+  </si>
+  <si>
+    <t>Bo</t>
   </si>
   <si>
     <t>Sherman</t>
@@ -6381,13 +6384,13 @@
         <v>120645.0</v>
       </c>
       <c r="J139" s="1" t="s">
-        <v>262</v>
+        <v>287</v>
       </c>
       <c r="K139" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="L139" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="140">
@@ -6419,7 +6422,7 @@
         <v>424144.0</v>
       </c>
       <c r="J140" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="K140" s="1" t="s">
         <v>90</v>
@@ -6442,7 +6445,7 @@
         <v>14</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="F141" s="1" t="s">
         <v>16</v>
@@ -6457,10 +6460,10 @@
         <v>221134.0</v>
       </c>
       <c r="J141" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="K141" s="1" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="142">
@@ -6492,10 +6495,10 @@
         <v>134321.0</v>
       </c>
       <c r="J142" s="1" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="K142" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="143">
@@ -6512,7 +6515,7 @@
         <v>14</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="F143" s="1" t="s">
         <v>16</v>
@@ -6527,13 +6530,13 @@
         <v>332444.0</v>
       </c>
       <c r="J143" s="1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="K143" s="1" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="L143" s="1" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="144">
@@ -6565,10 +6568,10 @@
         <v>564231.0</v>
       </c>
       <c r="J144" s="1" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="K144" s="1" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="145">
@@ -6585,7 +6588,7 @@
         <v>14</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="F145" s="1" t="s">
         <v>16</v>
@@ -6600,10 +6603,10 @@
         <v>250355.0</v>
       </c>
       <c r="J145" s="1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="K145" s="1" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="146">
@@ -6620,7 +6623,7 @@
         <v>14</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="F146" s="1" t="s">
         <v>16</v>
@@ -6635,7 +6638,7 @@
         <v>89405.0</v>
       </c>
       <c r="J146" s="1" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="K146" s="1" t="s">
         <v>172</v>
@@ -6670,10 +6673,10 @@
         <v>130669.0</v>
       </c>
       <c r="J147" s="1" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="K147" s="1" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="148">
@@ -6705,10 +6708,10 @@
         <v>309938.0</v>
       </c>
       <c r="J148" s="1" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="K148" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="149">
@@ -6740,7 +6743,7 @@
         <v>152565.0</v>
       </c>
       <c r="J149" s="1" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="K149" s="1" t="s">
         <v>135</v>
@@ -6760,7 +6763,7 @@
         <v>14</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="F150" s="1" t="s">
         <v>16</v>
@@ -6775,13 +6778,13 @@
         <v>430930.0</v>
       </c>
       <c r="J150" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="K150" s="1" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="L150" s="1" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="151">
@@ -6836,7 +6839,7 @@
         <v>14</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="F152" s="1" t="s">
         <v>16</v>
@@ -6851,10 +6854,10 @@
         <v>287612.0</v>
       </c>
       <c r="J152" s="1" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="K152" s="1" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="153">
@@ -6889,10 +6892,10 @@
         <v>46</v>
       </c>
       <c r="K153" s="1" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="L153" s="1" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="154">
@@ -6909,7 +6912,7 @@
         <v>14</v>
       </c>
       <c r="E154" s="1" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="F154" s="1" t="s">
         <v>16</v>
@@ -6927,7 +6930,7 @@
         <v>262</v>
       </c>
       <c r="K154" s="1" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="L154" s="1" t="s">
         <v>140</v>
@@ -6947,7 +6950,7 @@
         <v>14</v>
       </c>
       <c r="E155" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="F155" s="1" t="s">
         <v>16</v>
@@ -6965,7 +6968,7 @@
         <v>262</v>
       </c>
       <c r="K155" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="156">
@@ -6982,7 +6985,7 @@
         <v>14</v>
       </c>
       <c r="E156" s="1" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="F156" s="1" t="s">
         <v>16</v>
@@ -7000,7 +7003,7 @@
         <v>183</v>
       </c>
       <c r="K156" s="1" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="L156" s="1" t="s">
         <v>140</v>
@@ -7020,7 +7023,7 @@
         <v>14</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="F157" s="1" t="s">
         <v>16</v>
@@ -7058,7 +7061,7 @@
         <v>14</v>
       </c>
       <c r="E158" s="1" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="F158" s="1" t="s">
         <v>16</v>
@@ -7073,10 +7076,10 @@
         <v>109205.0</v>
       </c>
       <c r="J158" s="1" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="K158" s="1" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="159">
@@ -7093,7 +7096,7 @@
         <v>14</v>
       </c>
       <c r="E159" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="F159" s="1" t="s">
         <v>16</v>
@@ -7128,7 +7131,7 @@
         <v>14</v>
       </c>
       <c r="E160" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="F160" s="1" t="s">
         <v>16</v>
@@ -7143,13 +7146,13 @@
         <v>196635.0</v>
       </c>
       <c r="J160" s="1" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="K160" s="1" t="s">
         <v>99</v>
       </c>
       <c r="L160" s="1" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="161">
@@ -7166,7 +7169,7 @@
         <v>14</v>
       </c>
       <c r="E161" s="1" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="F161" s="1" t="s">
         <v>16</v>
@@ -7181,10 +7184,10 @@
         <v>191478.0</v>
       </c>
       <c r="J161" s="1" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="K161" s="1" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="L161" s="1" t="s">
         <v>178</v>
@@ -7219,10 +7222,10 @@
         <v>418086.0</v>
       </c>
       <c r="J162" s="1" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="K162" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="163">
@@ -7239,7 +7242,7 @@
         <v>14</v>
       </c>
       <c r="E163" s="1" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="F163" s="1" t="s">
         <v>16</v>
@@ -7254,10 +7257,10 @@
         <v>467422.0</v>
       </c>
       <c r="J163" s="1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="K163" s="1" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="L163" s="1" t="s">
         <v>140</v>
@@ -7277,7 +7280,7 @@
         <v>14</v>
       </c>
       <c r="E164" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="F164" s="1" t="s">
         <v>16</v>
@@ -7292,13 +7295,13 @@
         <v>48035.0</v>
       </c>
       <c r="J164" s="1" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="K164" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="L164" s="1" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="165">
@@ -7353,7 +7356,7 @@
         <v>14</v>
       </c>
       <c r="E166" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="F166" s="1" t="s">
         <v>16</v>
@@ -7371,7 +7374,7 @@
         <v>26</v>
       </c>
       <c r="K166" s="1" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="167">
@@ -7426,7 +7429,7 @@
         <v>14</v>
       </c>
       <c r="E168" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="F168" s="1" t="s">
         <v>16</v>
@@ -7441,10 +7444,10 @@
         <v>414893.0</v>
       </c>
       <c r="J168" s="1" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="K168" s="1" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="L168" s="1" t="s">
         <v>100</v>
@@ -7464,7 +7467,7 @@
         <v>14</v>
       </c>
       <c r="E169" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="F169" s="1" t="s">
         <v>16</v>
@@ -7479,7 +7482,7 @@
         <v>387142.0</v>
       </c>
       <c r="J169" s="1" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="K169" s="1" t="s">
         <v>151</v>
@@ -7499,7 +7502,7 @@
         <v>14</v>
       </c>
       <c r="E170" s="1" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="F170" s="1" t="s">
         <v>16</v>
@@ -7514,13 +7517,13 @@
         <v>480321.0</v>
       </c>
       <c r="J170" s="1" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="K170" s="1" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="L170" s="1" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="171">
@@ -7537,7 +7540,7 @@
         <v>14</v>
       </c>
       <c r="E171" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="F171" s="1" t="s">
         <v>16</v>
@@ -7552,10 +7555,10 @@
         <v>233064.0</v>
       </c>
       <c r="J171" s="1" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="K171" s="1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="L171" s="1" t="s">
         <v>178</v>
@@ -7575,7 +7578,7 @@
         <v>14</v>
       </c>
       <c r="E172" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="F172" s="1" t="s">
         <v>16</v>
@@ -7590,10 +7593,10 @@
         <v>565801.0</v>
       </c>
       <c r="J172" s="1" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="K172" s="1" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="173">
@@ -7610,7 +7613,7 @@
         <v>14</v>
       </c>
       <c r="E173" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="F173" s="1" t="s">
         <v>16</v>
@@ -7628,7 +7631,7 @@
         <v>23</v>
       </c>
       <c r="K173" s="1" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="174">
@@ -7645,7 +7648,7 @@
         <v>14</v>
       </c>
       <c r="E174" s="1" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="F174" s="1" t="s">
         <v>16</v>
@@ -7660,10 +7663,10 @@
         <v>198036.0</v>
       </c>
       <c r="J174" s="1" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="K174" s="1" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="L174" s="1" t="s">
         <v>121</v>
@@ -7715,13 +7718,13 @@
         <v>12</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D176" s="1" t="s">
         <v>78</v>
       </c>
       <c r="E176" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="F176" s="1" t="s">
         <v>16</v>
@@ -7736,10 +7739,10 @@
         <v>475220.0</v>
       </c>
       <c r="J176" s="1" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="K176" s="1" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="L176" s="1" t="s">
         <v>86</v>
@@ -7753,13 +7756,13 @@
         <v>12</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D177" s="1" t="s">
         <v>78</v>
       </c>
       <c r="E177" s="1" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="F177" s="1" t="s">
         <v>16</v>
@@ -7774,10 +7777,10 @@
         <v>519356.0</v>
       </c>
       <c r="J177" s="1" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="K177" s="1" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="178">
@@ -7788,13 +7791,13 @@
         <v>12</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D178" s="1" t="s">
         <v>78</v>
       </c>
       <c r="E178" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="F178" s="1" t="s">
         <v>16</v>
@@ -7809,10 +7812,10 @@
         <v>542884.0</v>
       </c>
       <c r="J178" s="1" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="K178" s="1" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="179">
@@ -7823,13 +7826,13 @@
         <v>12</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D179" s="1" t="s">
         <v>78</v>
       </c>
       <c r="E179" s="1" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="F179" s="1" t="s">
         <v>16</v>
@@ -7844,10 +7847,10 @@
         <v>540787.0</v>
       </c>
       <c r="J179" s="1" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="K179" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="L179" s="1" t="s">
         <v>136</v>
@@ -7861,13 +7864,13 @@
         <v>12</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D180" s="1" t="s">
         <v>78</v>
       </c>
       <c r="E180" s="1" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="F180" s="1" t="s">
         <v>16</v>
@@ -7882,10 +7885,10 @@
         <v>508143.0</v>
       </c>
       <c r="J180" s="1" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="K180" s="1" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row r="181">
@@ -7896,13 +7899,13 @@
         <v>12</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D181" s="1" t="s">
         <v>78</v>
       </c>
       <c r="E181" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="F181" s="1" t="s">
         <v>16</v>
@@ -7934,13 +7937,13 @@
         <v>12</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D182" s="1" t="s">
         <v>78</v>
       </c>
       <c r="E182" s="1" t="s">
-        <v>345</v>
+        <v>351</v>
       </c>
       <c r="F182" s="1" t="s">
         <v>16</v>
@@ -7972,13 +7975,13 @@
         <v>12</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D183" s="1" t="s">
         <v>78</v>
       </c>
       <c r="E183" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="F183" s="1" t="s">
         <v>16</v>
@@ -7993,10 +7996,10 @@
         <v>312884.0</v>
       </c>
       <c r="J183" s="1" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="K183" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="184">
@@ -8007,13 +8010,13 @@
         <v>12</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="D184" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E184" s="1" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="F184" s="1" t="s">
         <v>16</v>
@@ -8028,10 +8031,10 @@
         <v>460597.0</v>
       </c>
       <c r="J184" s="1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="K184" s="1" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="185">
@@ -8042,13 +8045,13 @@
         <v>12</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="D185" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E185" s="1" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="F185" s="1" t="s">
         <v>16</v>
@@ -8063,7 +8066,7 @@
         <v>489116.0</v>
       </c>
       <c r="J185" s="1" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="K185" s="1" t="s">
         <v>164</v>
@@ -8077,13 +8080,13 @@
         <v>12</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="D186" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E186" s="1" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="F186" s="1" t="s">
         <v>16</v>
@@ -8101,7 +8104,7 @@
         <v>40</v>
       </c>
       <c r="K186" s="1" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
     </row>
     <row r="187">
@@ -8112,13 +8115,13 @@
         <v>12</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="D187" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E187" s="1" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="F187" s="1" t="s">
         <v>16</v>
@@ -8133,10 +8136,10 @@
         <v>382731.0</v>
       </c>
       <c r="J187" s="1" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="K187" s="1" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
     <row r="188">
@@ -8147,13 +8150,13 @@
         <v>12</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="D188" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E188" s="1" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="F188" s="1" t="s">
         <v>16</v>
@@ -8168,7 +8171,7 @@
         <v>486284.0</v>
       </c>
       <c r="J188" s="1" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="K188" s="1" t="s">
         <v>164</v>
@@ -8185,13 +8188,13 @@
         <v>12</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="D189" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E189" s="1" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="F189" s="1" t="s">
         <v>16</v>
@@ -8206,13 +8209,13 @@
         <v>540096.0</v>
       </c>
       <c r="J189" s="1" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="K189" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="L189" s="1" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="190">
@@ -8223,13 +8226,13 @@
         <v>12</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="D190" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E190" s="1" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="F190" s="1" t="s">
         <v>16</v>
@@ -8247,7 +8250,7 @@
         <v>281</v>
       </c>
       <c r="K190" s="1" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="L190" s="1" t="s">
         <v>121</v>

</xml_diff>